<commit_message>
Made modifications to the code, this is the final version
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\suponugupati\IdeaProjects\OpenMRS_1\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57562789-E46B-4D1F-8793-7554C87D71E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D88D9638-01BF-4193-BB35-A94A808D8952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="LoginData" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
-  <si>
-    <t>Test Case ID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>username</t>
   </si>
@@ -36,38 +33,40 @@
     <t>password</t>
   </si>
   <si>
-    <t>T2</t>
-  </si>
-  <si>
     <t>admin</t>
   </si>
   <si>
     <t>Admin123</t>
   </si>
   <si>
-    <t>T3</t>
-  </si>
-  <si>
-    <t>T4</t>
-  </si>
-  <si>
-    <t>admin1</t>
-  </si>
-  <si>
-    <t>Admin1234</t>
+    <t>Scenario</t>
+  </si>
+  <si>
+    <t>valid credentials</t>
+  </si>
+  <si>
+    <t>Admin124</t>
+  </si>
+  <si>
+    <t>invalid credentials</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -87,14 +86,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{226454BB-26F0-441A-A4AC-9199AD8F5B28}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -372,72 +374,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.36328125" customWidth="1"/>
     <col min="2" max="2" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>